<commit_message>
Short Term Pf Update
</commit_message>
<xml_diff>
--- a/portfolios/portfolio-2025-06-02.xlsx
+++ b/portfolios/portfolio-2025-06-02.xlsx
@@ -76713,7 +76713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BO6"/>
+  <dimension ref="A1:BO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -77061,7 +77061,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>CNP</t>
+          <t>LMT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -77071,17 +77071,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CenterPoint Energy, Inc.</t>
+          <t>Lockheed Martin Corporation</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Industrials</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Utilities - Regulated Electric</t>
+          <t>Aerospace &amp; Defense</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -77091,122 +77091,122 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.centerpointenergy.com</t>
+          <t>https://www.lockheedmartin.com</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>24307591168</v>
+        <v>113019707392</v>
       </c>
       <c r="I2" t="n">
-        <v>44578607104</v>
+        <v>131520684032</v>
       </c>
       <c r="J2" t="n">
-        <v>649386429</v>
+        <v>172732348</v>
       </c>
       <c r="K2" t="n">
-        <v>652728000</v>
+        <v>234296000</v>
       </c>
       <c r="L2" t="n">
-        <v>25.16</v>
+        <v>20.79</v>
       </c>
       <c r="M2" t="n">
-        <v>21.4</v>
+        <v>17.16</v>
       </c>
       <c r="N2" t="n">
-        <v>2.72</v>
+        <v>1.57</v>
       </c>
       <c r="O2" t="n">
-        <v>2.22</v>
+        <v>16.82</v>
       </c>
       <c r="P2" t="n">
-        <v>13.26</v>
+        <v>15.14</v>
       </c>
       <c r="Q2" t="n">
-        <v>4.99</v>
+        <v>1.83</v>
       </c>
       <c r="R2" t="n">
-        <v>0.4514</v>
+        <v>0.1023</v>
       </c>
       <c r="S2" t="n">
-        <v>0.3759</v>
+        <v>0.121</v>
       </c>
       <c r="T2" t="n">
-        <v>0.2212</v>
+        <v>0.1269</v>
       </c>
       <c r="U2" t="n">
+        <v>0.0766</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="X2" t="n">
+        <v>71810998272</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>28.11</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="AC2" t="n">
         <v>0.108</v>
       </c>
-      <c r="V2" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="X2" t="n">
-        <v>8942999552</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.114</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>1.74</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>-0.182</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>-0.151</v>
-      </c>
       <c r="AD2" t="n">
-        <v>1916000000</v>
+        <v>1803000064</v>
       </c>
       <c r="AE2" t="n">
-        <v>22186999808</v>
+        <v>20303998976</v>
       </c>
       <c r="AF2" t="n">
-        <v>202.53</v>
+        <v>303.82</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.93</v>
+        <v>1.08</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.74</v>
+        <v>0.87</v>
       </c>
       <c r="AI2" t="n">
-        <v>16.78</v>
+        <v>28.68</v>
       </c>
       <c r="AJ2" t="n">
-        <v>-1248875008</v>
+        <v>5291125248</v>
       </c>
       <c r="AK2" t="n">
-        <v>2011000064</v>
+        <v>6745999872</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.0236</v>
+        <v>0.0274</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.132</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.0274</v>
+        <v>0.0265</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.5608</v>
+        <v>0.556</v>
       </c>
       <c r="AP2" t="n">
-        <v>37.24</v>
+        <v>482.38</v>
       </c>
       <c r="AQ2" t="n">
-        <v>38.44</v>
+        <v>524.23</v>
       </c>
       <c r="AR2" t="n">
-        <v>43</v>
+        <v>670</v>
       </c>
       <c r="AS2" t="n">
-        <v>32</v>
+        <v>408</v>
       </c>
       <c r="AT2" t="inlineStr">
         <is>
@@ -77214,75 +77214,75 @@
         </is>
       </c>
       <c r="AU2" t="n">
-        <v>2.47</v>
+        <v>2.29</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.58</v>
+        <v>0.29</v>
       </c>
       <c r="AW2" t="n">
-        <v>39.31</v>
+        <v>618.95</v>
       </c>
       <c r="AX2" t="n">
-        <v>25.41</v>
+        <v>418.88</v>
       </c>
       <c r="AY2" t="n">
-        <v>37.11</v>
+        <v>463.07</v>
       </c>
       <c r="AZ2" t="n">
-        <v>32.43</v>
+        <v>506.99</v>
       </c>
       <c r="BA2" t="n">
-        <v>5.59</v>
+        <v>1.59</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="BC2" t="n">
-        <v>0.328277365370141</v>
+        <v>0.4367724067801635</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.3946646719589237</v>
+        <v>0.529069603698733</v>
       </c>
       <c r="BE2" t="n">
-        <v>-0.1022959683814834</v>
+        <v>-0.1322285871366624</v>
       </c>
       <c r="BF2" t="n">
-        <v>1.560008364253685</v>
+        <v>1.802864722281068</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.1949571434703635</v>
+        <v>0.2146427305236873</v>
       </c>
       <c r="BH2" t="inlineStr">
         <is>
-          <t>EMA_Cross_Signal</t>
+          <t>SMA_Cross_Signal</t>
         </is>
       </c>
       <c r="BI2" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.6101</v>
+        <v>0.6124000000000001</v>
       </c>
       <c r="BK2" t="n">
         <v>0</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.5714</v>
+        <v>0.9286</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.2203</v>
+        <v>0.2247</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.5876</v>
+        <v>0.4822</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.5881999999999999</v>
+        <v>0.5621</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>LMT</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -77292,17 +77292,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lockheed Martin Corporation</t>
+          <t>Philip Morris International Inc.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Industrials</t>
+          <t>Consumer Defensive</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Aerospace &amp; Defense</t>
+          <t>Tobacco</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -77312,122 +77312,116 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.lockheedmartin.com</t>
+          <t>https://www.pmi.com</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>113019707392</v>
+        <v>281091932160</v>
       </c>
       <c r="I3" t="n">
-        <v>131520684032</v>
+        <v>328256421888</v>
       </c>
       <c r="J3" t="n">
-        <v>172732348</v>
+        <v>1552579194</v>
       </c>
       <c r="K3" t="n">
-        <v>234296000</v>
+        <v>1556519936</v>
       </c>
       <c r="L3" t="n">
-        <v>20.79</v>
+        <v>28.39</v>
       </c>
       <c r="M3" t="n">
-        <v>17.16</v>
+        <v>25.08</v>
       </c>
       <c r="N3" t="n">
-        <v>1.57</v>
+        <v>7.32</v>
       </c>
       <c r="O3" t="n">
-        <v>16.82</v>
+        <v>-25.78</v>
       </c>
       <c r="P3" t="n">
-        <v>15.14</v>
+        <v>20.21</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.83</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1023</v>
+        <v>0.6568000000000001</v>
       </c>
       <c r="S3" t="n">
-        <v>0.121</v>
+        <v>0.4231</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1269</v>
+        <v>0.4102</v>
       </c>
       <c r="U3" t="n">
-        <v>0.0766</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.83</v>
+        <v>0.198</v>
       </c>
       <c r="W3" t="n">
-        <v>0.08</v>
+        <v>0.14</v>
       </c>
       <c r="X3" t="n">
-        <v>71810998272</v>
+        <v>38385999872</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.045</v>
+        <v>0.058</v>
       </c>
       <c r="Z3" t="n">
-        <v>23.2</v>
+        <v>6.36</v>
       </c>
       <c r="AA3" t="n">
-        <v>28.11</v>
+        <v>7.2</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.139</v>
+        <v>0.247</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.108</v>
+        <v>0.252</v>
       </c>
       <c r="AD3" t="n">
-        <v>1803000064</v>
+        <v>4442999808</v>
       </c>
       <c r="AE3" t="n">
-        <v>20303998976</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>303.82</v>
+        <v>49633001472</v>
       </c>
       <c r="AG3" t="n">
-        <v>1.08</v>
+        <v>0.79</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.87</v>
+        <v>0.36</v>
       </c>
       <c r="AI3" t="n">
-        <v>28.68</v>
+        <v>-7</v>
       </c>
       <c r="AJ3" t="n">
-        <v>5291125248</v>
+        <v>8564250112</v>
       </c>
       <c r="AK3" t="n">
-        <v>6745999872</v>
+        <v>11626000384</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.0274</v>
+        <v>0.0299</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.132</v>
+        <v>0.05400000000000001</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.0265</v>
+        <v>0.051</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.556</v>
+        <v>0.8427</v>
       </c>
       <c r="AP3" t="n">
-        <v>482.38</v>
+        <v>180.59</v>
       </c>
       <c r="AQ3" t="n">
-        <v>524.23</v>
+        <v>176.03</v>
       </c>
       <c r="AR3" t="n">
-        <v>670</v>
+        <v>205</v>
       </c>
       <c r="AS3" t="n">
-        <v>408</v>
+        <v>143.45</v>
       </c>
       <c r="AT3" t="inlineStr">
         <is>
@@ -77435,717 +77429,69 @@
         </is>
       </c>
       <c r="AU3" t="n">
-        <v>2.29</v>
+        <v>1.94</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.29</v>
+        <v>0.54</v>
       </c>
       <c r="AW3" t="n">
-        <v>618.95</v>
+        <v>181.36</v>
       </c>
       <c r="AX3" t="n">
-        <v>418.88</v>
+        <v>98.93000000000001</v>
       </c>
       <c r="AY3" t="n">
-        <v>463.07</v>
+        <v>164.63</v>
       </c>
       <c r="AZ3" t="n">
-        <v>506.99</v>
+        <v>138.62</v>
       </c>
       <c r="BA3" t="n">
-        <v>1.59</v>
+        <v>2.06</v>
       </c>
       <c r="BB3" t="n">
         <v>0.01</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.4367721444232255</v>
+        <v>0.3890788202554054</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.5290692765197731</v>
+        <v>0.4697632656478883</v>
       </c>
       <c r="BE3" t="n">
-        <v>-0.1322287919896218</v>
+        <v>-0.2340932813559296</v>
       </c>
       <c r="BF3" t="n">
-        <v>1.802863637331443</v>
+        <v>1.524161478899244</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.2146427613217923</v>
+        <v>0.2348302634625276</v>
       </c>
       <c r="BH3" t="inlineStr">
-        <is>
-          <t>SMA_Cross_Signal</t>
-        </is>
-      </c>
-      <c r="BI3" t="n">
-        <v>12</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>0.615</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>0.9167</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>0.4886</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>0.5632</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>NVR</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-06-02</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>NVR, Inc.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Consumer Cyclical</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Residential Construction</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://www.nvrinc.com</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>20805769216</v>
-      </c>
-      <c r="I4" t="n">
-        <v>19696087040</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2879740</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2923830</v>
-      </c>
-      <c r="L4" t="n">
-        <v>14.66</v>
-      </c>
-      <c r="M4" t="n">
-        <v>13.74</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1.94</v>
-      </c>
-      <c r="O4" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="P4" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1.83</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.1949</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.1681</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.1477</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="X4" t="n">
-        <v>10742590464</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>485.31</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>518.05</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>-0.185</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>-0.24</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>2176901888</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>1067212992</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>26.99</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>1343.02</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>1303018240</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>1435784960</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>7115.93</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>7700</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>8000</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>7200</v>
-      </c>
-      <c r="AT4" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-      <c r="AV4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>9964.77</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>6562.85</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>7165.62</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>8258.34</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>4.92</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>0.3759825057301134</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>0.4535388017578115</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>-0.1034153210925537</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>1.469325253221376</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>0.23738622692343</v>
-      </c>
-      <c r="BH4" t="inlineStr">
-        <is>
-          <t>SMA_Cross_Signal</t>
-        </is>
-      </c>
-      <c r="BI4" t="n">
-        <v>3</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>0.6592</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>0.3185</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>0.4474</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>0.5626</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-06-02</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Philip Morris International Inc.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Consumer Defensive</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Tobacco</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>https://www.pmi.com</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>281091932160</v>
-      </c>
-      <c r="I5" t="n">
-        <v>328256421888</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1552579194</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1556519936</v>
-      </c>
-      <c r="L5" t="n">
-        <v>28.39</v>
-      </c>
-      <c r="M5" t="n">
-        <v>25.08</v>
-      </c>
-      <c r="N5" t="n">
-        <v>7.32</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-25.78</v>
-      </c>
-      <c r="P5" t="n">
-        <v>20.21</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>8.550000000000001</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.6568000000000001</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.4231</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.4102</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.198</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="X5" t="n">
-        <v>38385999872</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>6.36</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.247</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.252</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>4442999808</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>49633001472</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>-7</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>8564250112</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>11626000384</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0.0299</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0.05400000000000001</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.051</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0.8427</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>180.59</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>176.03</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>205</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>143.45</v>
-      </c>
-      <c r="AT5" t="inlineStr">
-        <is>
-          <t>buy</t>
-        </is>
-      </c>
-      <c r="AU5" t="n">
-        <v>1.94</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>181.36</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>98.93000000000001</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>164.63</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>138.62</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>2.06</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>0.3890788862322949</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>0.4697633474502576</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>-0.2340932669020119</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>1.52416183215601</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>0.234830236161383</v>
-      </c>
-      <c r="BH5" t="inlineStr">
         <is>
           <t>EMA_Cross_Signal</t>
         </is>
       </c>
-      <c r="BI5" t="n">
-        <v>132</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>0.6204</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>0.0152</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>0.6894</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>0.2409</v>
-      </c>
-      <c r="BN5" t="n">
-        <v>0.4946</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>0.5571</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>VTR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-06-02</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Ventas, Inc.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Real Estate</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>REIT - Healthcare Facilities</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://www.ventasreit.com</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>29009434624</v>
-      </c>
-      <c r="I6" t="n">
-        <v>42128576512</v>
-      </c>
-      <c r="J6" t="n">
-        <v>448960515</v>
-      </c>
-      <c r="K6" t="n">
-        <v>451297984</v>
-      </c>
-      <c r="L6" t="n">
-        <v>194.79</v>
-      </c>
-      <c r="M6" t="n">
-        <v>401.75</v>
-      </c>
-      <c r="N6" t="n">
-        <v>5.74</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2.53</v>
-      </c>
-      <c r="P6" t="n">
-        <v>21.85</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.4218</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.3814</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.1415</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.0282</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="X6" t="n">
-        <v>5055948800</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0.141</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>182335008</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>12921492480</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>108.9</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>25.43</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>869675776</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>1384321024</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0.0299</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0.0192</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0.0385</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>5.5455</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>64.28</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>75.95</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>83</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>69</v>
-      </c>
-      <c r="AT6" t="inlineStr">
-        <is>
-          <t>buy</t>
-        </is>
-      </c>
-      <c r="AU6" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="AV6" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>71.36</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>49.06</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>66.54000000000001</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>63.73</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>0.4181128471837579</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>0.5058257735633864</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>-0.09485908637293616</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>1.809146380837495</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>0.205621626403174</v>
-      </c>
-      <c r="BH6" t="inlineStr">
-        <is>
-          <t>SMA_Cross_Signal</t>
-        </is>
-      </c>
-      <c r="BI6" t="n">
-        <v>7</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>0.5838</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>0.4286</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>0.1676</v>
-      </c>
-      <c r="BN6" t="n">
-        <v>0.4383</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>0.5562</v>
+      <c r="BI3" t="n">
+        <v>131</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.6205000000000001</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.0153</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.6870000000000001</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.2411</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0.5582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>